<commit_message>
Aggiunte colonne vaccinati > 4-6 mesi, vaccinati < 4-6 mesi
Signed-off-by: enricocid <enrico2588@gmail.com>
</commit_message>
<xml_diff>
--- a/dati/data_iss_età_2021-07-14.xlsx
+++ b/dati/data_iss_età_2021-07-14.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>casi non vaccinati</t>
   </si>
@@ -23,48 +23,72 @@
     <t>casi vaccinati 1 dose</t>
   </si>
   <si>
-    <t>casi vaccinati</t>
+    <t>casi vaccinati &gt; 4-6 mesi</t>
+  </si>
+  <si>
+    <t>casi vaccinati &lt; 4-6 mesi</t>
   </si>
   <si>
     <t>casi booster</t>
   </si>
   <si>
+    <t>casi vaccinati completo</t>
+  </si>
+  <si>
     <t>ospedalizzati non vaccinati</t>
   </si>
   <si>
     <t>ospedalizzati vaccinati 1 dose</t>
   </si>
   <si>
-    <t>ospedalizzati vaccinati</t>
+    <t>ospedalizzati vaccinati &gt; 4-6 mesi</t>
+  </si>
+  <si>
+    <t>ospedalizzati vaccinati &lt; 4-6 mesi</t>
   </si>
   <si>
     <t>ospedalizzati booster</t>
   </si>
   <si>
+    <t>ospedalizzati vaccinati completo</t>
+  </si>
+  <si>
     <t>terapia intensiva non vaccinati</t>
   </si>
   <si>
     <t>terapia intensiva vaccinati 1 dose</t>
   </si>
   <si>
-    <t>terapia intensiva vaccinati</t>
+    <t>terapia intensiva vaccinati &gt; 4-6 mesi</t>
+  </si>
+  <si>
+    <t>terapia intensiva vaccinati &lt; 4-6 mesi</t>
   </si>
   <si>
     <t>terapia intensiva booster</t>
   </si>
   <si>
+    <t>terapia intensiva vaccinati completo</t>
+  </si>
+  <si>
     <t>decessi non vaccinati</t>
   </si>
   <si>
     <t>decessi vaccinati 1 dose</t>
   </si>
   <si>
-    <t>decessi vaccinati</t>
+    <t>decessi vaccinati &gt; 4-6 mesi</t>
+  </si>
+  <si>
+    <t>decessi vaccinati &lt; 4-6 mesi</t>
   </si>
   <si>
     <t>decessi booster</t>
   </si>
   <si>
+    <t>decessi vaccinati completo</t>
+  </si>
+  <si>
     <t>età</t>
   </si>
   <si>
@@ -80,22 +104,22 @@
     <t>80+</t>
   </si>
   <si>
-    <t>casi vaccinati completo</t>
-  </si>
-  <si>
-    <t>casi vaccinati booster</t>
-  </si>
-  <si>
     <t>ospedalizzati/ti non vaccinati</t>
   </si>
   <si>
     <t>ospedalizzati/ti vaccinati 1 dose</t>
   </si>
   <si>
-    <t>ospedalizzati/ti vaccinati</t>
+    <t>ospedalizzati/ti vaccinati &gt; 4-6 mesi</t>
+  </si>
+  <si>
+    <t>ospedalizzati/ti vaccinati &lt; 4-6 mesi</t>
   </si>
   <si>
     <t>ospedalizzati/ti booster</t>
+  </si>
+  <si>
+    <t>ospedalizzati/ti vaccinati completo</t>
   </si>
 </sst>
 </file>
@@ -453,15 +477,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -511,10 +535,34 @@
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>13549</v>
@@ -523,51 +571,75 @@
         <v>1243</v>
       </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <v>528</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
+      <c r="H2">
         <v>513</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>11</v>
       </c>
-      <c r="H2">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
         <v>4</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
+      <c r="N2">
         <v>13</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
         <v>7</v>
       </c>
-      <c r="O2">
+      <c r="U2">
         <v>1</v>
       </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:25">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>5747</v>
@@ -576,51 +648,75 @@
         <v>1586</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <v>727</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="H3">
         <v>779</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>51</v>
       </c>
-      <c r="H3">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
         <v>24</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
+      <c r="N3">
         <v>66</v>
       </c>
-      <c r="K3">
+      <c r="O3">
         <v>3</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
         <v>45</v>
       </c>
-      <c r="O3">
+      <c r="U3">
         <v>4</v>
       </c>
-      <c r="P3">
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
         <v>1</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:25">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>1491</v>
@@ -629,51 +725,75 @@
         <v>1067</v>
       </c>
       <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>568</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
+      <c r="H4">
         <v>420</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>151</v>
       </c>
-      <c r="H4">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
         <v>70</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
+      <c r="N4">
         <v>47</v>
       </c>
-      <c r="K4">
+      <c r="O4">
         <v>17</v>
       </c>
-      <c r="L4">
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
         <v>2</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
+      <c r="T4">
         <v>158</v>
       </c>
-      <c r="O4">
+      <c r="U4">
         <v>46</v>
       </c>
-      <c r="P4">
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
         <v>12</v>
       </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:25">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>302</v>
@@ -682,46 +802,70 @@
         <v>58</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>487</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="H5">
         <v>168</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>27</v>
       </c>
-      <c r="H5">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
         <v>142</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
+      <c r="N5">
         <v>21</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
         <v>5</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
+      <c r="T5">
         <v>147</v>
       </c>
-      <c r="O5">
+      <c r="U5">
         <v>21</v>
       </c>
-      <c r="P5">
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
         <v>55</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -731,15 +875,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -748,39 +892,57 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="B2">
         <v>14011891</v>
@@ -789,17 +951,17 @@
         <v>1815895</v>
       </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <v>1607769</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
       <c r="H2">
         <v>0</v>
       </c>
@@ -818,10 +980,28 @@
       <c r="M2">
         <v>0</v>
       </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>9340510</v>
@@ -830,17 +1010,17 @@
         <v>5502988</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <v>3603962</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
       <c r="H3">
         <v>0</v>
       </c>
@@ -859,10 +1039,28 @@
       <c r="M3">
         <v>0</v>
       </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:19">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>3251872</v>
@@ -871,17 +1069,17 @@
         <v>5415352</v>
       </c>
       <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>4905555</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
       <c r="H4">
         <v>0</v>
       </c>
@@ -900,10 +1098,28 @@
       <c r="M4">
         <v>0</v>
       </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>460790</v>
@@ -912,17 +1128,17 @@
         <v>281202</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>3812115</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
       <c r="H5">
         <v>0</v>
       </c>
@@ -939,6 +1155,24 @@
         <v>0</v>
       </c>
       <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
         <v>0</v>
       </c>
     </row>

</xml_diff>